<commit_message>
Updated Courses.xlsx with the additional modules (and their scheduled allocations)
</commit_message>
<xml_diff>
--- a/ifs-solver/src/main/resources/input/2020-Sem1-CAES-Wvl/Courses.xlsx
+++ b/ifs-solver/src/main/resources/input/2020-Sem1-CAES-Wvl/Courses.xlsx
@@ -5,27 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha\Documents\CS Honours\COMP700 - HP\student-lab-sectioning\ifs-solver\src\main\resources\input\CAES-2020-Sem1-Wvl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha\Documents\CS Honours\COMP700 - HP\student-lab-sectioning\ifs-solver\src\main\resources\input\2020-Sem1-CAES-Wvl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8557C2B1-ADA9-4574-91EB-04E478B66148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95318FE6-4CF7-47EB-80B4-7CC74F0994D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="60" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
   <si>
     <t>course</t>
   </si>
@@ -94,6 +103,30 @@
   </si>
   <si>
     <t>STAT130</t>
+  </si>
+  <si>
+    <t>BIOL103</t>
+  </si>
+  <si>
+    <t>BIOL195</t>
+  </si>
+  <si>
+    <t>BIOL196</t>
+  </si>
+  <si>
+    <t>GEOG110</t>
+  </si>
+  <si>
+    <t>MATH140</t>
+  </si>
+  <si>
+    <t>MATH196</t>
+  </si>
+  <si>
+    <t>PHYS113</t>
+  </si>
+  <si>
+    <t>PHYS195</t>
   </si>
 </sst>
 </file>
@@ -411,11 +444,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -544,7 +575,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -553,13 +584,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -567,22 +598,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -590,13 +621,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -605,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -619,10 +650,10 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -642,10 +673,10 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -665,13 +696,13 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>144</v>
@@ -682,22 +713,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>192</v>
+        <v>144</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -705,22 +736,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
       <c r="F13">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -728,22 +759,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -751,22 +782,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>48</v>
+        <v>192</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -774,16 +805,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -803,10 +834,10 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -820,22 +851,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
       <c r="F18">
-        <v>250</v>
+        <v>48</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -843,13 +874,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -858,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="F19">
-        <v>250</v>
+        <v>48</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -866,22 +897,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <v>2</v>
       </c>
       <c r="F20">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -889,22 +920,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
       <c r="F21">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -912,22 +943,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E22">
         <v>2</v>
       </c>
       <c r="F22">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -935,7 +966,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -944,13 +975,13 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="F23">
-        <v>154</v>
+        <v>260</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -958,22 +989,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
       <c r="F24">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -981,22 +1012,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E25">
         <v>2</v>
       </c>
       <c r="F25">
-        <v>491</v>
+        <v>40</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1004,22 +1035,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26">
-        <v>350</v>
+        <v>40</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1027,22 +1058,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27">
-        <v>491</v>
+        <v>154</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1050,22 +1081,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28">
-        <v>750</v>
+        <v>136</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -1079,16 +1110,16 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -1102,16 +1133,16 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E30">
         <v>2</v>
       </c>
       <c r="F30">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1119,22 +1150,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
       <c r="F31">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -1142,22 +1173,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E32">
         <v>2</v>
       </c>
       <c r="F32">
-        <v>320</v>
+        <v>165</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -1165,22 +1196,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33">
-        <v>320</v>
+        <v>491</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -1188,22 +1219,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>320</v>
+        <v>350</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -1211,16 +1242,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -1234,13 +1265,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>10</v>
@@ -1249,9 +1280,193 @@
         <v>1</v>
       </c>
       <c r="F36">
+        <v>106</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>320</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>270</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>320</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>320</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>320</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>320</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>491</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
         <v>544</v>
       </c>
-      <c r="G36">
+      <c r="G44">
         <v>1</v>
       </c>
     </row>

</xml_diff>